<commit_message>
Intermediate version. Working, hopping 30 channels. Packet length = 7 bytes, channels 11-41, bitrate 38.4kBit/s. New RF settings added.
</commit_message>
<xml_diff>
--- a/Tirusse/tirusse.xlsx
+++ b/Tirusse/tirusse.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Timings</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Baudrate</t>
   </si>
   <si>
-    <t>kBit/s</t>
-  </si>
-  <si>
     <t>Bit length</t>
   </si>
   <si>
@@ -49,6 +46,27 @@
   </si>
   <si>
     <t>mS</t>
+  </si>
+  <si>
+    <t>Bit/s</t>
+  </si>
+  <si>
+    <t>Real packet duration</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>Experimental</t>
+  </si>
+  <si>
+    <t>Receive duration</t>
+  </si>
+  <si>
+    <t>*2</t>
+  </si>
+  <si>
+    <t>30 channels duration</t>
   </si>
 </sst>
 </file>
@@ -56,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -160,13 +178,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
@@ -472,89 +491,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C9"/>
+  <dimension ref="A3:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>4.8</v>
+        <v>10000</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>32</v>
       </c>
       <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="B6" s="2">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3">
         <f>8*(B5+B6)</f>
-        <v>304</v>
+        <v>616</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <f>1000000/B4</f>
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5">
-        <f>1000/B4</f>
-        <v>208.33333333333334</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="5">
         <f>B7*B8/1000</f>
-        <v>63.333333333333336</v>
+        <v>61.6</v>
       </c>
       <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2">
+        <v>38400</v>
+      </c>
+      <c r="C14" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3">
+        <f>8*(B15+B16)</f>
+        <v>616</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="5">
+        <f>1000000/B14</f>
+        <v>26.041666666666668</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5">
+        <f>B17*B18/1000</f>
+        <v>16.041666666666668</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="6">
+        <f>B19</f>
+        <v>16.041666666666668</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <f>B21*2</f>
+        <v>32.083333333333336</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24">
+        <f>B23*30</f>
+        <v>962.50000000000011</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM added, some calculations added in XLSX
</commit_message>
<xml_diff>
--- a/Tirusse/tirusse.xlsx
+++ b/Tirusse/tirusse.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>Timings</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>30 channels duration</t>
+  </si>
+  <si>
+    <t>Подбор</t>
   </si>
 </sst>
 </file>
@@ -493,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +543,9 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -607,7 +613,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="2">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -618,10 +624,13 @@
         <v>7</v>
       </c>
       <c r="B16" s="2">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,7 +639,7 @@
       </c>
       <c r="B17" s="3">
         <f>8*(B15+B16)</f>
-        <v>616</v>
+        <v>256</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -654,7 +663,7 @@
       </c>
       <c r="B19" s="5">
         <f>B17*B18/1000</f>
-        <v>16.041666666666668</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -665,8 +674,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="6">
-        <f>B19</f>
-        <v>16.041666666666668</v>
+        <v>6.8</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -681,7 +689,7 @@
       </c>
       <c r="B23">
         <f>B21*2</f>
-        <v>32.083333333333336</v>
+        <v>13.6</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -696,7 +704,7 @@
       </c>
       <c r="B24">
         <f>B23*30</f>
-        <v>962.50000000000011</v>
+        <v>408</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Working, but idle mode consumpts ~7 mA.
</commit_message>
<xml_diff>
--- a/Tirusse/tirusse.xlsx
+++ b/Tirusse/tirusse.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Timings</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>Подбор</t>
+  </si>
+  <si>
+    <t>RX_OFF duration</t>
+  </si>
+  <si>
+    <t>RX_ON duration</t>
+  </si>
+  <si>
+    <t>ON/OFF ratio</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>*1.5</t>
   </si>
 </sst>
 </file>
@@ -494,15 +509,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D24"/>
+  <dimension ref="A3:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -683,6 +699,21 @@
         <v>13</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <f>B21*1.5</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
@@ -698,16 +729,50 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="2">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="2">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B24">
-        <f>B23*30</f>
-        <v>408</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B27" s="4">
+        <f>(B25+B26)*30</f>
+        <v>1890</v>
+      </c>
+      <c r="C27" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="5">
+        <f>100*B26/(B26+B25)</f>
+        <v>28.571428571428573</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CC powerdown implemented, average current ~4mA.
</commit_message>
<xml_diff>
--- a/Tirusse/tirusse.xlsx
+++ b/Tirusse/tirusse.xlsx
@@ -512,7 +512,7 @@
   <dimension ref="A3:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,10 +700,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4">
         <f>B21*1.5</f>
         <v>10.199999999999999</v>
       </c>
@@ -715,10 +715,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <f>B21*2</f>
         <v>13.6</v>
       </c>
@@ -734,7 +734,7 @@
         <v>18</v>
       </c>
       <c r="B25" s="2">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -757,7 +757,7 @@
       </c>
       <c r="B27" s="4">
         <f>(B25+B26)*30</f>
-        <v>1890</v>
+        <v>3780</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -769,7 +769,7 @@
       </c>
       <c r="B28" s="5">
         <f>100*B26/(B26+B25)</f>
-        <v>28.571428571428573</v>
+        <v>14.285714285714286</v>
       </c>
       <c r="C28" t="s">
         <v>21</v>

</xml_diff>